<commit_message>
updated files and code
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Huang_1996.xlsx
+++ b/ISRaD_data_files/Huang_1996.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20386"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfromm\Documents\GitHub\ISRaD_SvF\ISRaD_data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82F468BE-8C90-4F98-A592-386C8F9C86FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="11560" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="11556" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="997">
   <si>
     <t>entry_name</t>
   </si>
@@ -3011,12 +3017,21 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>pro_usda_soil_order</t>
+  </si>
+  <si>
+    <t>Spodosols</t>
+  </si>
+  <si>
+    <t>Inceptisols</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3143,10 +3158,18 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_layer" xfId="5"/>
+    <cellStyle name="Normal_layer" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3428,14 +3451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3485,7 +3508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3570,7 +3593,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3623,20 +3646,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="45.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3682,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3682,7 +3705,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3699,7 +3722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3728,21 +3751,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="35.83203125" customWidth="1"/>
-    <col min="21" max="21" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="22" max="22" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3783,76 +3806,79 @@
         <v>86</v>
       </c>
       <c r="N1" t="s">
+        <v>994</v>
+      </c>
+      <c r="O1" t="s">
         <v>87</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>91</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>92</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>93</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>94</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>95</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>96</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>97</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>99</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>100</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>101</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>102</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>103</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>104</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>105</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>106</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>107</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>108</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3892,77 +3918,77 @@
       <c r="M2" t="s">
         <v>118</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>119</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>120</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>122</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>123</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>124</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>125</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>126</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>127</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>128</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>132</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>133</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>134</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>135</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>136</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>137</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>138</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>139</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>140</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3990,29 +4016,26 @@
       <c r="M3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>147</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>148</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>149</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>146</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>150</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>151</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>152</v>
-      </c>
-      <c r="V3" t="s">
-        <v>153</v>
       </c>
       <c r="W3" t="s">
         <v>153</v>
@@ -4021,43 +4044,46 @@
         <v>153</v>
       </c>
       <c r="Y3" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z3" t="s">
         <v>154</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>155</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>156</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>157</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>158</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>159</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>150</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>160</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>161</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>162</v>
       </c>
       <c r="AI3" t="s">
         <v>162</v>
       </c>
       <c r="AJ3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4073,17 +4099,17 @@
       <c r="H4" t="s">
         <v>164</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>165</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>166</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4100,19 +4126,22 @@
         <v>164</v>
       </c>
       <c r="N5" t="s">
+        <v>995</v>
+      </c>
+      <c r="O5" t="s">
         <v>169</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>165</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>166</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4129,19 +4158,22 @@
         <v>164</v>
       </c>
       <c r="N6" t="s">
+        <v>996</v>
+      </c>
+      <c r="O6" t="s">
         <v>171</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>165</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>166</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -4158,19 +4190,22 @@
         <v>164</v>
       </c>
       <c r="N7" t="s">
+        <v>996</v>
+      </c>
+      <c r="O7" t="s">
         <v>171</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>165</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>166</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4187,19 +4222,22 @@
         <v>164</v>
       </c>
       <c r="N8" t="s">
+        <v>995</v>
+      </c>
+      <c r="O8" t="s">
         <v>169</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>165</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>166</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4216,15 +4254,18 @@
         <v>164</v>
       </c>
       <c r="N9" t="s">
+        <v>996</v>
+      </c>
+      <c r="O9" t="s">
         <v>171</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>165</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>166</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4240,14 +4281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4360,7 +4401,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4470,7 +4511,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4562,16 +4603,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CT37"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:98">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4867,7 +4908,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:98">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5163,7 +5204,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:98">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5402,7 +5443,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:98">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5437,7 +5478,7 @@
         <v>5.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:98">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5472,7 +5513,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:98">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5507,7 +5548,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:98">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5542,7 +5583,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:98">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5577,7 +5618,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:98">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5612,7 +5653,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:98">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -5647,7 +5688,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:98">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5682,7 +5723,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:98">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -5717,7 +5758,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:98">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -5752,7 +5793,7 @@
         <v>6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:98">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -5787,7 +5828,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:98">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -5822,7 +5863,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:98">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -5857,7 +5898,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:56">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -5892,7 +5933,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:56">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -5927,7 +5968,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:56">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -5962,7 +6003,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:56">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -5997,7 +6038,7 @@
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:56">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -6032,7 +6073,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:56">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -6067,7 +6108,7 @@
         <v>3.4999999999999996E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:56">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -6102,7 +6143,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:56">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -6137,7 +6178,7 @@
         <v>5.5000000000000005E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:56">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -6172,7 +6213,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:56">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -6207,7 +6248,7 @@
         <v>3.9000000000000003E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -6242,7 +6283,7 @@
         <v>3.9000000000000003E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -6277,7 +6318,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -6312,7 +6353,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -6347,7 +6388,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -6382,7 +6423,7 @@
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:56">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -6417,7 +6458,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:56">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -6452,7 +6493,7 @@
         <v>2.8000000000000004E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:56">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -6487,7 +6528,7 @@
         <v>3.9000000000000003E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:56">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -6522,7 +6563,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:56">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -6557,7 +6598,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:56">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -6604,14 +6645,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6697,7 +6738,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6780,7 +6821,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6839,16 +6880,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="52">
+    <row r="1" spans="1:73" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7069,7 +7110,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -7287,7 +7328,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7466,14 +7507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7565,7 +7606,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -7648,7 +7689,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -7707,14 +7748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AR21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>749</v>
       </c>
@@ -7848,7 +7889,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -7982,7 +8023,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
         <v>795</v>
       </c>
@@ -8005,7 +8046,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>800</v>
       </c>
@@ -8139,7 +8180,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>833</v>
       </c>
@@ -8252,7 +8293,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="6" spans="1:44">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>866</v>
       </c>
@@ -8353,7 +8394,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="7" spans="1:44">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>893</v>
       </c>
@@ -8427,7 +8468,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="8" spans="1:44">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>913</v>
       </c>
@@ -8495,7 +8536,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>930</v>
       </c>
@@ -8548,7 +8589,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="10" spans="1:44">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>946</v>
       </c>
@@ -8580,7 +8621,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="11" spans="1:44">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>956</v>
       </c>
@@ -8606,7 +8647,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="12" spans="1:44">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>963</v>
       </c>
@@ -8623,7 +8664,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="13" spans="1:44">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U13" t="s">
         <v>968</v>
       </c>
@@ -8637,7 +8678,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U14" t="s">
         <v>972</v>
       </c>
@@ -8648,7 +8689,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U15" t="s">
         <v>975</v>
       </c>
@@ -8659,7 +8700,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="U16" t="s">
         <v>978</v>
       </c>
@@ -8670,7 +8711,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="17" spans="40:41">
+    <row r="17" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN17" t="s">
         <v>981</v>
       </c>
@@ -8678,7 +8719,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="18" spans="40:41">
+    <row r="18" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN18" t="s">
         <v>983</v>
       </c>
@@ -8686,7 +8727,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="19" spans="40:41">
+    <row r="19" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN19" t="s">
         <v>985</v>
       </c>
@@ -8694,7 +8735,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="20" spans="40:41">
+    <row r="20" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN20" t="s">
         <v>987</v>
       </c>
@@ -8702,7 +8743,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="21" spans="40:41">
+    <row r="21" spans="40:41" x14ac:dyDescent="0.3">
       <c r="AN21" t="s">
         <v>989</v>
       </c>

</xml_diff>